<commit_message>
add data validation checks/controls in data engine
Change-Id: I2a85b7e30ba9658db45736f847cd35b0694d6663
Signed-off-by: dell <dell@dell-PC>
</commit_message>
<xml_diff>
--- a/PhpTravelsKWD/src/dataEngine/DataEngine.xlsx
+++ b/PhpTravelsKWD/src/dataEngine/DataEngine.xlsx
@@ -4,19 +4,26 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="135" windowWidth="20115" windowHeight="7485" activeTab="2"/>
+    <workbookView windowHeight="2460" windowWidth="10755" xWindow="0" yWindow="2520"/>
   </bookViews>
   <sheets>
-    <sheet name="TestSteps" sheetId="1" r:id="rId1"/>
-    <sheet name="TestCases" sheetId="2" r:id="rId2"/>
-    <sheet name="Settings" sheetId="3" r:id="rId3"/>
+    <sheet name="TestSteps" r:id="rId1" sheetId="1"/>
+    <sheet name="TestCases" r:id="rId2" sheetId="2"/>
+    <sheet name="Settings" r:id="rId3" sheetId="3"/>
   </sheets>
+  <definedNames>
+    <definedName name="Account_Login">Settings!$C$2:$C$10</definedName>
+    <definedName name="Action_Keyword">Settings!$E$2:$E$10</definedName>
+    <definedName name="Home_Page">Settings!$B$2:$B$10</definedName>
+    <definedName name="My_Account">Settings!$D$2:$D$10</definedName>
+    <definedName name="Page_Names">Settings!$A$2:$A$10</definedName>
+  </definedNames>
   <calcPr calcId="125725"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="82" uniqueCount="59">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="131" uniqueCount="61">
   <si>
     <t>Test_ID</t>
   </si>
@@ -174,15 +181,6 @@
     <t>@phpTravels1-2</t>
   </si>
   <si>
-    <t>FAIL</t>
-  </si>
-  <si>
-    <t>IE</t>
-  </si>
-  <si>
-    <t>Page_Name</t>
-  </si>
-  <si>
     <t>Home_Page_Obj</t>
   </si>
   <si>
@@ -192,13 +190,29 @@
     <t>Home_Page</t>
   </si>
   <si>
-    <t>Login_Page</t>
+    <t>Chrome</t>
+  </si>
+  <si>
+    <t>Action_Keyword</t>
+  </si>
+  <si>
+    <t>Page_Names</t>
+  </si>
+  <si>
+    <t>Account_Login</t>
+  </si>
+  <si>
+    <t>My_Account</t>
+  </si>
+  <si>
+    <t>My_Account_Obj</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <numFmts count="0"/>
   <fonts count="3">
     <font>
       <sz val="11"/>
@@ -256,23 +270,23 @@
     </border>
   </borders>
   <cellStyleXfs count="2">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
+    <xf applyAlignment="0" applyBorder="0" applyFill="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="0" fontId="2" numFmtId="0">
       <alignment vertical="top"/>
       <protection locked="0"/>
     </xf>
   </cellStyleXfs>
   <cellXfs count="6">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyBorder="1"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="1" applyFont="1" borderId="1" fillId="0" fontId="1" numFmtId="0" xfId="0"/>
+    <xf applyBorder="1" borderId="1" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="1" applyFill="1" applyFont="1" borderId="1" fillId="0" fontId="1" numFmtId="0" xfId="0"/>
+    <xf applyAlignment="1" applyBorder="1" applyProtection="1" borderId="1" fillId="0" fontId="2" numFmtId="0" xfId="1"/>
+    <xf applyBorder="1" borderId="1" fillId="0" fontId="0" numFmtId="0" quotePrefix="1" xfId="0"/>
   </cellXfs>
   <cellStyles count="2">
-    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle builtinId="8" name="Hyperlink" xfId="1"/>
+    <cellStyle builtinId="0" name="Normal" xfId="0"/>
   </cellStyles>
   <dxfs count="2">
     <dxf>
@@ -298,10 +312,10 @@
       </fill>
     </dxf>
   </dxfs>
-  <tableStyles count="1" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16">
-    <tableStyle name="MySqlDefault" pivot="0" table="0" count="2">
-      <tableStyleElement type="wholeTable" dxfId="1"/>
-      <tableStyleElement type="headerRow" dxfId="0"/>
+  <tableStyles count="1" defaultPivotStyle="PivotStyleLight16" defaultTableStyle="TableStyleMedium9">
+    <tableStyle count="2" name="MySqlDefault" pivot="0" table="0">
+      <tableStyleElement dxfId="1" type="wholeTable"/>
+      <tableStyleElement dxfId="0" type="headerRow"/>
     </tableStyle>
   </tableStyles>
 </styleSheet>
@@ -312,10 +326,10 @@
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
-        <a:sysClr val="windowText" lastClr="000000"/>
+        <a:sysClr lastClr="000000" val="windowText"/>
       </a:dk1>
       <a:lt1>
-        <a:sysClr val="window" lastClr="FFFFFF"/>
+        <a:sysClr lastClr="FFFFFF" val="window"/>
       </a:lt1>
       <a:dk2>
         <a:srgbClr val="1F497D"/>
@@ -471,7 +485,7 @@
         </a:gradFill>
       </a:fillStyleLst>
       <a:lnStyleLst>
-        <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln algn="ctr" cap="flat" cmpd="sng" w="9525">
           <a:solidFill>
             <a:schemeClr val="phClr">
               <a:shade val="95000"/>
@@ -480,13 +494,13 @@
           </a:solidFill>
           <a:prstDash val="solid"/>
         </a:ln>
-        <a:ln w="25400" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln algn="ctr" cap="flat" cmpd="sng" w="25400">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
         </a:ln>
-        <a:ln w="38100" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln algn="ctr" cap="flat" cmpd="sng" w="38100">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
@@ -496,7 +510,7 @@
       <a:effectStyleLst>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw blurRad="40000" dist="20000" dir="5400000" rotWithShape="0">
+            <a:outerShdw blurRad="40000" dir="5400000" dist="20000" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="38000"/>
               </a:srgbClr>
@@ -505,7 +519,7 @@
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
+            <a:outerShdw blurRad="40000" dir="5400000" dist="23000" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="35000"/>
               </a:srgbClr>
@@ -514,7 +528,7 @@
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
+            <a:outerShdw blurRad="40000" dir="5400000" dist="23000" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="35000"/>
               </a:srgbClr>
@@ -524,12 +538,12 @@
             <a:camera prst="orthographicFront">
               <a:rot lat="0" lon="0" rev="0"/>
             </a:camera>
-            <a:lightRig rig="threePt" dir="t">
+            <a:lightRig dir="t" rig="threePt">
               <a:rot lat="0" lon="0" rev="1200000"/>
             </a:lightRig>
           </a:scene3d>
           <a:sp3d>
-            <a:bevelT w="63500" h="25400"/>
+            <a:bevelT h="25400" w="63500"/>
           </a:sp3d>
         </a:effectStyle>
       </a:effectStyleLst>
@@ -560,7 +574,7 @@
             </a:gs>
           </a:gsLst>
           <a:path path="circle">
-            <a:fillToRect l="50000" t="-80000" r="50000" b="180000"/>
+            <a:fillToRect b="180000" l="50000" r="50000" t="-80000"/>
           </a:path>
         </a:gradFill>
         <a:gradFill rotWithShape="1">
@@ -579,7 +593,7 @@
             </a:gs>
           </a:gsLst>
           <a:path path="circle">
-            <a:fillToRect l="50000" t="50000" r="50000" b="50000"/>
+            <a:fillToRect b="50000" l="50000" r="50000" t="50000"/>
           </a:path>
         </a:gradFill>
       </a:bgFillStyleLst>
@@ -592,23 +606,24 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:G11"/>
+  <dimension ref="A1:I11"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F2" sqref="F2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D16" sqref="D16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="8.7109375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="11.7109375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="35.7109375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="33" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="16" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="19.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="8.7109375" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="11.7109375" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="35.7109375" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" width="35.7109375" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" width="33.0" collapsed="true"/>
+    <col min="6" max="6" bestFit="true" customWidth="true" width="16.0" collapsed="true"/>
+    <col min="7" max="7" bestFit="true" customWidth="true" width="19.7109375" collapsed="true"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7">
+    <row r="1" spans="1:8">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -619,19 +634,22 @@
         <v>2</v>
       </c>
       <c r="D1" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="E1" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="G1" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="G1" s="3" t="s">
+      <c r="H1" s="3" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="2" spans="1:7">
+    <row r="2" spans="1:8">
       <c r="A2" s="2" t="s">
         <v>10</v>
       </c>
@@ -641,18 +659,21 @@
       <c r="C2" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="D2" s="2"/>
-      <c r="E2" s="2" t="s">
+      <c r="D2" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="E2" s="2"/>
+      <c r="F2" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="F2" s="2" t="s">
-        <v>53</v>
-      </c>
       <c r="G2" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="H2" s="2" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="3" spans="1:7">
+    <row r="3" spans="1:8">
       <c r="A3" s="2" t="s">
         <v>10</v>
       </c>
@@ -662,16 +683,19 @@
       <c r="C3" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="D3" s="2"/>
-      <c r="E3" s="2" t="s">
+      <c r="D3" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="E3" s="2"/>
+      <c r="F3" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="F3" s="2"/>
-      <c r="G3" s="2" t="s">
+      <c r="G3" s="2"/>
+      <c r="H3" s="2" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="4" spans="1:7">
+    <row r="4" spans="1:8">
       <c r="A4" s="2" t="s">
         <v>10</v>
       </c>
@@ -682,17 +706,20 @@
         <v>6</v>
       </c>
       <c r="D4" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="E4" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="E4" s="2" t="s">
+      <c r="F4" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="F4" s="2"/>
-      <c r="G4" s="2" t="s">
+      <c r="G4" s="2"/>
+      <c r="H4" s="2" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="5" spans="1:7">
+    <row r="5" spans="1:8">
       <c r="A5" s="2" t="s">
         <v>10</v>
       </c>
@@ -703,19 +730,22 @@
         <v>7</v>
       </c>
       <c r="D5" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="E5" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="E5" s="2" t="s">
+      <c r="F5" s="2" t="s">
         <v>49</v>
       </c>
-      <c r="F5" s="4" t="s">
+      <c r="G5" s="4" t="s">
         <v>50</v>
       </c>
-      <c r="G5" s="2" t="s">
+      <c r="H5" s="2" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="6" spans="1:7">
+    <row r="6" spans="1:8">
       <c r="A6" s="2" t="s">
         <v>10</v>
       </c>
@@ -726,19 +756,22 @@
         <v>8</v>
       </c>
       <c r="D6" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="E6" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="E6" s="2" t="s">
+      <c r="F6" s="2" t="s">
         <v>49</v>
       </c>
-      <c r="F6" s="5" t="s">
+      <c r="G6" s="5" t="s">
         <v>51</v>
       </c>
-      <c r="G6" s="2" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7">
+      <c r="H6" s="2" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8">
       <c r="A7" s="2" t="s">
         <v>10</v>
       </c>
@@ -749,17 +782,20 @@
         <v>9</v>
       </c>
       <c r="D7" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="E7" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="E7" s="2" t="s">
+      <c r="F7" s="2" t="s">
         <v>43</v>
       </c>
-      <c r="F7" s="2"/>
-      <c r="G7" s="2" t="s">
+      <c r="G7" s="2"/>
+      <c r="H7" s="2" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="8" spans="1:7">
+    <row r="8" spans="1:8">
       <c r="A8" s="2" t="s">
         <v>10</v>
       </c>
@@ -770,15 +806,16 @@
         <v>31</v>
       </c>
       <c r="D8" s="2"/>
-      <c r="E8" s="2" t="s">
+      <c r="E8" s="2"/>
+      <c r="F8" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="F8" s="2"/>
-      <c r="G8" s="2" t="s">
+      <c r="G8" s="2"/>
+      <c r="H8" s="2" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="9" spans="1:7">
+    <row r="9" spans="1:8">
       <c r="A9" s="2" t="s">
         <v>10</v>
       </c>
@@ -789,17 +826,20 @@
         <v>32</v>
       </c>
       <c r="D9" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="E9" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="E9" s="2" t="s">
+      <c r="F9" s="2" t="s">
         <v>44</v>
       </c>
-      <c r="F9" s="2"/>
-      <c r="G9" s="2" t="s">
+      <c r="G9" s="2"/>
+      <c r="H9" s="2" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="10" spans="1:7">
+    <row r="10" spans="1:8">
       <c r="A10" s="2" t="s">
         <v>10</v>
       </c>
@@ -810,17 +850,20 @@
         <v>33</v>
       </c>
       <c r="D10" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="E10" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="E10" s="2" t="s">
+      <c r="F10" s="2" t="s">
         <v>45</v>
       </c>
-      <c r="F10" s="2"/>
-      <c r="G10" s="2" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="11" spans="1:7">
+      <c r="G10" s="2"/>
+      <c r="H10" s="2" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8">
       <c r="A11" s="2" t="s">
         <v>10</v>
       </c>
@@ -831,34 +874,46 @@
         <v>34</v>
       </c>
       <c r="D11" s="2"/>
-      <c r="E11" s="2" t="s">
+      <c r="E11" s="2"/>
+      <c r="F11" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="F11" s="2"/>
-      <c r="G11" s="2" t="s">
+      <c r="G11" s="2"/>
+      <c r="H11" s="2" t="s">
         <v>47</v>
       </c>
     </row>
   </sheetData>
+  <dataValidations count="3">
+    <dataValidation allowBlank="1" showErrorMessage="1" showInputMessage="1" sqref="D2:D11" type="list">
+      <formula1>Page_Names</formula1>
+    </dataValidation>
+    <dataValidation allowBlank="1" showErrorMessage="1" showInputMessage="1" sqref="E2:E11" type="list">
+      <formula1>INDIRECT(D2)</formula1>
+    </dataValidation>
+    <dataValidation allowBlank="1" showErrorMessage="1" showInputMessage="1" sqref="F2:F11" type="list">
+      <formula1>Action_Keyword</formula1>
+    </dataValidation>
+  </dataValidations>
   <hyperlinks>
-    <hyperlink ref="F5" r:id="rId1"/>
+    <hyperlink r:id="rId1" ref="G5"/>
   </hyperlinks>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
   <pageSetup orientation="portrait" r:id="rId2"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:D4"/>
+  <dimension ref="A1:E4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="I11" sqref="I11"/>
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="2" max="2" width="32.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="32.42578125" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4">
@@ -886,7 +941,7 @@
         <v>40</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>52</v>
+        <v>47</v>
       </c>
     </row>
     <row r="3" spans="1:4">
@@ -908,58 +963,145 @@
       <c r="D4" s="2"/>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:C4"/>
+  <dimension ref="A1:F10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="11.5703125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="15.85546875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="15.28515625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="15.28515625" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="24.28515625" collapsed="true"/>
+    <col min="3" max="4" customWidth="true" width="24.28515625" collapsed="true"/>
+    <col min="5" max="5" bestFit="true" customWidth="true" width="15.85546875" collapsed="true"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3">
+    <row r="1" spans="1:5">
       <c r="A1" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5">
+      <c r="A2" s="2" t="s">
         <v>54</v>
       </c>
-      <c r="B1" s="1" t="s">
-        <v>55</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3">
-      <c r="A2" s="2" t="s">
-        <v>57</v>
-      </c>
-      <c r="B2" s="2"/>
-      <c r="C2" s="2"/>
-    </row>
-    <row r="3" spans="1:3">
+      <c r="B2" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="E2" s="2" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5">
       <c r="A3" s="2" t="s">
         <v>58</v>
       </c>
       <c r="B3" s="2"/>
-      <c r="C3" s="2"/>
-    </row>
-    <row r="4" spans="1:3">
-      <c r="A4" s="2"/>
+      <c r="C3" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="E3" s="2" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5">
+      <c r="A4" s="2" t="s">
+        <v>59</v>
+      </c>
       <c r="B4" s="2"/>
-      <c r="C4" s="2"/>
+      <c r="C4" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="D4" s="2"/>
+      <c r="E4" s="2" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5">
+      <c r="A5" s="2"/>
+      <c r="B5" s="2"/>
+      <c r="C5" s="2"/>
+      <c r="D5" s="2"/>
+      <c r="E5" s="2" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5">
+      <c r="A6" s="2"/>
+      <c r="B6" s="2"/>
+      <c r="C6" s="2"/>
+      <c r="D6" s="2"/>
+      <c r="E6" s="2" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5">
+      <c r="A7" s="2"/>
+      <c r="B7" s="2"/>
+      <c r="C7" s="2"/>
+      <c r="D7" s="2"/>
+      <c r="E7" s="2" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5">
+      <c r="A8" s="2"/>
+      <c r="B8" s="2"/>
+      <c r="C8" s="2"/>
+      <c r="D8" s="2"/>
+      <c r="E8" s="2" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5">
+      <c r="A9" s="2"/>
+      <c r="B9" s="2"/>
+      <c r="C9" s="2"/>
+      <c r="D9" s="2"/>
+      <c r="E9" s="2" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5">
+      <c r="A10" s="2"/>
+      <c r="B10" s="2"/>
+      <c r="C10" s="2"/>
+      <c r="D10" s="2"/>
+      <c r="E10" s="2" t="s">
+        <v>19</v>
+      </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>